<commit_message>
changed start_date size -1y to -4y
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -136,115 +136,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Natijalar Grafigi</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'Data'!B1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Data'!$A$2:$A$13</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Data'!$B$2:$B$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>4</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -534,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,137 +436,16 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>region</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>SUM(balance)</t>
+          <t>SUM(t.amount)</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Andijon</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>22285325.24452801</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Buxoro</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>19452496.53911553</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Fargona</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>23519281.75152642</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Jizzax</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>20403964.7086287</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Namangan</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>16495362.67715254</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Navoiy</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>22113535.96970741</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Qashqadaryo</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>24279845.85770413</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Samarqand</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>21058654.85822927</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Sirdaryo</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>18184362.06925693</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Surxandaryo</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>20649613.83273836</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Toshkent</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>19599057.11325114</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Xorazm</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>22060592.43089294</v>
+      <c r="A2" t="n">
+        <v>-10110.3343329413</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>